<commit_message>
add plot for comparsion with baselines
</commit_message>
<xml_diff>
--- a/plot/layerwiseOverhead/layerwise_overhead.xlsx
+++ b/plot/layerwiseOverhead/layerwise_overhead.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuboluo/Documents/PycharmProjects/SmartSwitch/plot/layer-wise inference time/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuboluo/Documents/PycharmProjects/SmartSwitch/plot/layerwiseOverhead/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4084AE-EE66-4C46-A1B0-C605DF77B92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB9301E-F3BE-FC44-B1A5-57F70A81B082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="-18080" windowWidth="28040" windowHeight="16080" activeTab="1" xr2:uid="{4E70910A-5F71-D846-B62A-5D4F7FC823D7}"/>
+    <workbookView xWindow="300" yWindow="1740" windowWidth="21120" windowHeight="12740" activeTab="1" xr2:uid="{4E70910A-5F71-D846-B62A-5D4F7FC823D7}"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +128,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -141,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -149,6 +155,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,7 +619,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,24 +634,24 @@
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3">
@@ -665,7 +672,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3">
@@ -686,7 +693,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3">
@@ -707,7 +714,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3">
@@ -728,7 +735,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="3">
@@ -749,7 +756,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3">
@@ -779,24 +786,24 @@
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="2">
@@ -813,7 +820,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="2">
@@ -830,7 +837,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2">
@@ -847,7 +854,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="2">
@@ -864,7 +871,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="2">
@@ -881,7 +888,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="2">
@@ -898,7 +905,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="2">

</xml_diff>